<commit_message>
Changed standard error calculations for fold change and relative-survival to reflect the appropriate propagation of errors
</commit_message>
<xml_diff>
--- a/XTT data - FBS Experiment/FBS Titration XTT Assays.xlsx
+++ b/XTT data - FBS Experiment/FBS Titration XTT Assays.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchicagoedu-my.sharepoint.com/personal/clozano_uchicago_edu/Documents/College/internships/Renal Diseases/data/EV Experiment 4-2025/Copy for Github/XTT Assays/FBS Titration 3-2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchicagoedu-my.sharepoint.com/personal/clozano_uchicago_edu/Documents/College/internships/Renal Diseases/data/2024/XTT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="745" documentId="8_{313F682C-816C-4341-BD9F-6296F97FCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ECB6BBB-7551-43D5-94BD-0F2F670D59F7}"/>
+  <xr:revisionPtr revIDLastSave="744" documentId="8_{313F682C-816C-4341-BD9F-6296F97FCAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B19C7871-F592-4074-A539-93B22DAA5D4D}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="2" xr2:uid="{7004FC09-E616-41FE-8413-71351939002C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="5" xr2:uid="{7004FC09-E616-41FE-8413-71351939002C}"/>
   </bookViews>
   <sheets>
     <sheet name="2hr" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="48hr" sheetId="8" r:id="rId3"/>
     <sheet name="72hr" sheetId="9" r:id="rId4"/>
     <sheet name="All corrected absorbances" sheetId="7" r:id="rId5"/>
+    <sheet name="Fold changes (from R code)" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t>BLK</t>
   </si>
@@ -52,6 +53,30 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>Serum condition</t>
+  </si>
+  <si>
+    <t>Confidence interval</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Mean log2-fold change</t>
+  </si>
+  <si>
+    <t>log2-fold change confidence interval calculated via Wilcoxon signed-rank test, which assumes the log2-fold change measurements have symmetric, but not necessarily normal, distributions</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>HSA + 0.0%</t>
   </si>
 </sst>
 </file>
@@ -106,12 +131,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="26">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -161,6 +195,108 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color auto="1"/>
+      </right>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="mediumDashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -231,49 +367,157 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -320,6 +564,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -648,33 +896,33 @@
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.69140625" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.3828125" style="20" customWidth="1"/>
     <col min="3" max="9" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="16">
+      <c r="B1" s="19">
         <v>490</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="16">
         <v>0.1</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="16">
         <v>0</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="16">
         <v>0.01</v>
       </c>
-      <c r="I1" s="15">
+      <c r="I1" s="18">
         <v>0.02</v>
       </c>
     </row>
@@ -794,55 +1042,55 @@
       </c>
     </row>
     <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="6">
+      <c r="C7" s="9">
         <v>0.46100000000000002</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="10">
         <v>0.86199999999999999</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="10">
         <v>0.83799999999999997</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="10">
         <v>0.82899999999999996</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="10">
         <v>0.86499999999999999</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="10">
         <v>0.92</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="11">
         <v>0.82199999999999995</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="9" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="16">
+      <c r="B9" s="19">
         <v>630</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="12">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="13">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="13">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="13">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="13">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="14">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
@@ -937,31 +1185,31 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="6">
+      <c r="C14" s="9">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="10">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="10">
         <v>0.06</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="10">
         <v>0.06</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="10">
         <v>6.2E-2</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="11">
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C16">
@@ -1144,14 +1392,14 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C23">
         <f>C16-AVERAGE($C$16:$C$21)</f>
         <v>2.5166666666666671E-2</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="47">
         <f t="shared" ref="D23:I23" si="2">D16-AVERAGE($C$16:$C$21)</f>
         <v>0.15916666666666673</v>
       </c>
@@ -1346,33 +1594,33 @@
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.69140625" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.3828125" style="20" customWidth="1"/>
     <col min="3" max="9" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="16">
+      <c r="B1" s="19">
         <v>490</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="16">
         <v>0.1</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="16">
         <v>0</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="16">
         <v>0.01</v>
       </c>
-      <c r="I1" s="15">
+      <c r="I1" s="18">
         <v>0.02</v>
       </c>
     </row>
@@ -1492,52 +1740,52 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="6">
+      <c r="C7" s="9">
         <v>0.40600000000000003</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="10">
         <v>1.2689999999999999</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="10">
         <v>0.81799999999999995</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="10">
         <v>0.85399999999999998</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="10">
         <v>0.99399999999999999</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="10">
         <v>1.2430000000000001</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="11">
         <v>1.0029999999999999</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="9" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="16">
+      <c r="B9" s="19">
         <v>630</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="12">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="13">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="13">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="13">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="13">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="14">
         <v>6.2E-2</v>
       </c>
     </row>
@@ -1634,31 +1882,31 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="6">
+      <c r="C14" s="9">
         <v>0.06</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="10">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="10">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="10">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="11">
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C16">
@@ -1841,7 +2089,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C23">
@@ -2038,686 +2286,686 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A5213B-810F-4023-B0D8-1F6A0A86459D}">
   <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.69140625" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.3828125" style="20" customWidth="1"/>
     <col min="3" max="9" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="16">
+      <c r="B1" s="19">
         <v>490</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="16">
         <v>0.1</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="16">
         <v>0</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="16">
         <v>0.01</v>
       </c>
-      <c r="I1" s="15">
+      <c r="I1" s="18">
         <v>0.02</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C2" s="18">
+      <c r="C2" s="21">
         <v>0.40799999999999997</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="22">
         <v>1.5209999999999999</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="22">
         <v>0.877</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="22">
         <v>0.876</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="22">
         <v>1.28</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="22">
         <v>1.1559999999999999</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="23">
         <v>1.395</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C3" s="18">
+      <c r="C3" s="21">
         <v>0.40300000000000002</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="22">
         <v>1.728</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="22">
         <v>1.0129999999999999</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="22">
         <v>0.93600000000000005</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="22">
         <v>1.41</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="22">
         <v>1.194</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="23">
         <v>1.427</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C4" s="18">
+      <c r="C4" s="21">
         <v>0.40600000000000003</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="22">
         <v>1.6140000000000001</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="22">
         <v>0.86</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="22">
         <v>0.95</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="22">
         <v>1.383</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="22">
         <v>1.3260000000000001</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="23">
         <v>1.4410000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C5" s="18">
+      <c r="C5" s="21">
         <v>0.39800000000000002</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="22">
         <v>1.625</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="22">
         <v>0.86099999999999999</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="22">
         <v>0.88200000000000001</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="22">
         <v>1.4339999999999999</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="22">
         <v>1.226</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="23">
         <v>1.46</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C6" s="18">
+      <c r="C6" s="21">
         <v>0.40400000000000003</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="22">
         <v>1.627</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="22">
         <v>0.91600000000000004</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="22">
         <v>0.79</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="22">
         <v>1.1419999999999999</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="22">
         <v>1.266</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="23">
         <v>1.526</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="21">
+      <c r="C7" s="24">
         <v>0.40300000000000002</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="25">
         <v>1.657</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="25">
         <v>0.93400000000000005</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="25">
         <v>1.0329999999999999</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="25">
         <v>1.175</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="25">
         <v>1.393</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="26">
         <v>1.409</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="9" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="16">
+      <c r="B9" s="19">
         <v>630</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="27">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="28">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="28">
         <v>0.05</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="28">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="28">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="28">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="29">
         <v>0.06</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C10" s="18">
+      <c r="C10" s="21">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="22">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="22">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="22">
         <v>0.05</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="22">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="22">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="23">
         <v>6.2E-2</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C11" s="18">
+      <c r="C11" s="21">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="22">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="22">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="22">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="22">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="22">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="23">
         <v>0.06</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C12" s="18">
+      <c r="C12" s="21">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="22">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="22">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="22">
         <v>0.05</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="22">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="22">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="23">
         <v>0.06</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C13" s="18">
+      <c r="C13" s="21">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="22">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="22">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="22">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="22">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="22">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="23">
         <v>6.2E-2</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="21">
+      <c r="C14" s="24">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="25">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="25">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="25">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="25">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="25">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="26">
         <v>6.3E-2</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="22">
         <f>C2-C9</f>
         <v>0.35</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="22">
         <f t="shared" ref="D16:I16" si="0">D2-D9</f>
         <v>1.446</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="22">
         <f t="shared" si="0"/>
         <v>0.82699999999999996</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="22">
         <f t="shared" si="0"/>
         <v>0.82499999999999996</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="22">
         <f t="shared" si="0"/>
         <v>1.2210000000000001</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="22">
         <f t="shared" si="0"/>
         <v>1.099</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="22">
         <f t="shared" si="0"/>
         <v>1.335</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C17" s="19">
+      <c r="C17" s="22">
         <f t="shared" ref="C17:I21" si="1">C3-C10</f>
         <v>0.34600000000000003</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="22">
         <f t="shared" si="1"/>
         <v>1.6519999999999999</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="22">
         <f t="shared" si="1"/>
         <v>0.96199999999999986</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="22">
         <f t="shared" si="1"/>
         <v>0.88600000000000001</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="22">
         <f t="shared" si="1"/>
         <v>1.353</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="22">
         <f t="shared" si="1"/>
         <v>1.135</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="22">
         <f t="shared" si="1"/>
         <v>1.365</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C18" s="19">
+      <c r="C18" s="22">
         <f t="shared" si="1"/>
         <v>0.35000000000000003</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="22">
         <f t="shared" si="1"/>
         <v>1.538</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="22">
         <f t="shared" si="1"/>
         <v>0.80899999999999994</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="22">
         <f t="shared" si="1"/>
         <v>0.89899999999999991</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="22">
         <f t="shared" si="1"/>
         <v>1.3260000000000001</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="22">
         <f t="shared" si="1"/>
         <v>1.268</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="22">
         <f t="shared" si="1"/>
         <v>1.381</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C19" s="19">
+      <c r="C19" s="22">
         <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="22">
         <f t="shared" si="1"/>
         <v>1.548</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="22">
         <f t="shared" si="1"/>
         <v>0.80999999999999994</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="22">
         <f t="shared" si="1"/>
         <v>0.83199999999999996</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="22">
         <f t="shared" si="1"/>
         <v>1.3779999999999999</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="22">
         <f t="shared" si="1"/>
         <v>1.17</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="22">
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C20" s="19">
+      <c r="C20" s="22">
         <f t="shared" si="1"/>
         <v>0.34500000000000003</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="22">
         <f t="shared" si="1"/>
         <v>1.552</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="22">
         <f t="shared" si="1"/>
         <v>0.86699999999999999</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="22">
         <f t="shared" si="1"/>
         <v>0.74099999999999999</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="22">
         <f t="shared" si="1"/>
         <v>1.0859999999999999</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="22">
         <f t="shared" si="1"/>
         <v>1.2070000000000001</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="22">
         <f t="shared" si="1"/>
         <v>1.464</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C21" s="19">
+      <c r="C21" s="22">
         <f t="shared" si="1"/>
         <v>0.34600000000000003</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="22">
         <f t="shared" si="1"/>
         <v>1.5820000000000001</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="22">
         <f t="shared" si="1"/>
         <v>0.88300000000000001</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="22">
         <f t="shared" si="1"/>
         <v>0.98199999999999987</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="22">
         <f t="shared" si="1"/>
         <v>1.119</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="22">
         <f t="shared" si="1"/>
         <v>1.335</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="22">
         <f t="shared" si="1"/>
         <v>1.3460000000000001</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="22">
         <f>C16-AVERAGE($C$16:$C$21)</f>
         <v>3.8333333333332997E-3</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="22">
         <f t="shared" ref="D23:I23" si="2">D16-AVERAGE($C$16:$C$21)</f>
         <v>1.0998333333333332</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="22">
         <f t="shared" si="2"/>
         <v>0.48083333333333328</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="22">
         <f t="shared" si="2"/>
         <v>0.47883333333333328</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="22">
         <f t="shared" si="2"/>
         <v>0.87483333333333335</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="22">
         <f t="shared" si="2"/>
         <v>0.75283333333333324</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="22">
         <f t="shared" si="2"/>
         <v>0.98883333333333323</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C24" s="19">
+      <c r="C24" s="22">
         <f t="shared" ref="C24:I28" si="3">C17-AVERAGE($C$16:$C$21)</f>
         <v>-1.6666666666664831E-4</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="22">
         <f t="shared" si="3"/>
         <v>1.3058333333333332</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="22">
         <f t="shared" si="3"/>
         <v>0.61583333333333323</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="22">
         <f t="shared" si="3"/>
         <v>0.53983333333333339</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="22">
         <f t="shared" si="3"/>
         <v>1.0068333333333332</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="22">
         <f t="shared" si="3"/>
         <v>0.78883333333333328</v>
       </c>
-      <c r="I24" s="19">
+      <c r="I24" s="22">
         <f t="shared" si="3"/>
         <v>1.0188333333333333</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C25" s="19">
+      <c r="C25" s="22">
         <f t="shared" si="3"/>
         <v>3.8333333333333552E-3</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="22">
         <f t="shared" si="3"/>
         <v>1.1918333333333333</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="22">
         <f t="shared" si="3"/>
         <v>0.46283333333333326</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="22">
         <f t="shared" si="3"/>
         <v>0.55283333333333329</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="22">
         <f t="shared" si="3"/>
         <v>0.97983333333333333</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H25" s="22">
         <f t="shared" si="3"/>
         <v>0.92183333333333328</v>
       </c>
-      <c r="I25" s="19">
+      <c r="I25" s="22">
         <f t="shared" si="3"/>
         <v>1.0348333333333333</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C26" s="19">
+      <c r="C26" s="22">
         <f t="shared" si="3"/>
         <v>-6.1666666666666536E-3</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="22">
         <f t="shared" si="3"/>
         <v>1.2018333333333333</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="22">
         <f t="shared" si="3"/>
         <v>0.46383333333333326</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="22">
         <f t="shared" si="3"/>
         <v>0.48583333333333328</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="22">
         <f t="shared" si="3"/>
         <v>1.0318333333333332</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="22">
         <f t="shared" si="3"/>
         <v>0.8238333333333332</v>
       </c>
-      <c r="I26" s="19">
+      <c r="I26" s="22">
         <f t="shared" si="3"/>
         <v>1.0538333333333332</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C27" s="19">
+      <c r="C27" s="22">
         <f t="shared" si="3"/>
         <v>-1.1666666666666492E-3</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="22">
         <f t="shared" si="3"/>
         <v>1.2058333333333333</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="22">
         <f t="shared" si="3"/>
         <v>0.52083333333333326</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="22">
         <f t="shared" si="3"/>
         <v>0.39483333333333331</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="22">
         <f t="shared" si="3"/>
         <v>0.73983333333333312</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="22">
         <f t="shared" si="3"/>
         <v>0.86083333333333334</v>
       </c>
-      <c r="I27" s="19">
+      <c r="I27" s="22">
         <f t="shared" si="3"/>
         <v>1.1178333333333332</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C28" s="19">
+      <c r="C28" s="22">
         <f t="shared" si="3"/>
         <v>-1.6666666666664831E-4</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="22">
         <f t="shared" si="3"/>
         <v>1.2358333333333333</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="22">
         <f t="shared" si="3"/>
         <v>0.53683333333333327</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="22">
         <f t="shared" si="3"/>
         <v>0.63583333333333325</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="22">
         <f t="shared" si="3"/>
         <v>0.77283333333333326</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="22">
         <f t="shared" si="3"/>
         <v>0.98883333333333323</v>
       </c>
-      <c r="I28" s="19">
+      <c r="I28" s="22">
         <f t="shared" si="3"/>
         <v>0.99983333333333335</v>
       </c>
@@ -2744,319 +2992,319 @@
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.69140625" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="16.3828125" style="20" customWidth="1"/>
     <col min="3" max="9" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="16">
+      <c r="B1" s="19">
         <v>490</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13">
+      <c r="D1" s="16">
         <v>0.1</v>
       </c>
-      <c r="E1" s="13">
+      <c r="E1" s="16">
         <v>0</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="17">
         <v>1E-3</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H1" s="13">
+      <c r="H1" s="16">
         <v>0.01</v>
       </c>
-      <c r="I1" s="15">
+      <c r="I1" s="18">
         <v>0.02</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C2" s="18">
+      <c r="C2" s="21">
         <v>0.43</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="22">
         <v>1.8169999999999999</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="22">
         <v>0.877</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="22">
         <v>0.96799999999999997</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="22">
         <v>1.157</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="22">
         <v>1.4610000000000001</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="23">
         <v>1.383</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C3" s="18">
+      <c r="C3" s="21">
         <v>0.41199999999999998</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="22">
         <v>1.532</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="22">
         <v>1.1539999999999999</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="22">
         <v>0.88100000000000001</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="22">
         <v>1.6359999999999999</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="22">
         <v>1.2749999999999999</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="23">
         <v>1.38</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C4" s="18">
+      <c r="C4" s="21">
         <v>0.42899999999999999</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="22">
         <v>1.6479999999999999</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="22">
         <v>0.99399999999999999</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="22">
         <v>1.2030000000000001</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="22">
         <v>1.2789999999999999</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="22">
         <v>1.284</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="23">
         <v>1.603</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C5" s="18">
+      <c r="C5" s="21">
         <v>0.41499999999999998</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="22">
         <v>1.73</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="22">
         <v>0.95</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="22">
         <v>1.0529999999999999</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="22">
         <v>1.446</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="22">
         <v>1.2090000000000001</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="23">
         <v>1.4910000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C6" s="18">
+      <c r="C6" s="21">
         <v>0.42499999999999999</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="22">
         <v>1.67</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="22">
         <v>0.83099999999999996</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="22">
         <v>1.105</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="22">
         <v>1.3839999999999999</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="22">
         <v>1.514</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="23">
         <v>1.671</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C7" s="21">
+      <c r="C7" s="24">
         <v>0.443</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="25">
         <v>1.8320000000000001</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="25">
         <v>1.0720000000000001</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="25">
         <v>1.04</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="25">
         <v>1.4370000000000001</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="25">
         <v>1.39</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="26">
         <v>1.5069999999999999</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="9" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="16">
+      <c r="B9" s="19">
         <v>630</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="27">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="28">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="28">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="28">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="28">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="28">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="29">
         <v>6.2E-2</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C10" s="18">
+      <c r="C10" s="21">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="50">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="50">
         <v>0.05</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="50">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="50">
         <v>5.5E-2</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="50">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="23">
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C11" s="18">
+      <c r="C11" s="21">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="50">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="50">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="50">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="50">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="50">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="23">
         <v>0.06</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C12" s="18">
+      <c r="C12" s="21">
         <v>5.5E-2</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="22">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="22">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="22">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="22">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="22">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="23">
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="C13" s="18">
+      <c r="C13" s="21">
         <v>0.06</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="22">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="22">
         <v>4.7E-2</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="22">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="22">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="22">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="23">
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="21">
+      <c r="C14" s="24">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="25">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="25">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="25">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="25">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="25">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="I14" s="23">
+      <c r="I14" s="26">
         <v>6.2E-2</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C16">
@@ -3239,7 +3487,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C23">
@@ -3479,7 +3727,7 @@
         <f>'2hr'!C23</f>
         <v>2.5166666666666671E-2</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="47">
         <f>'2hr'!D23</f>
         <v>0.15916666666666673</v>
       </c>
@@ -4267,4 +4515,640 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EB5B07-2C62-407D-998B-3C85DEE01623}">
+  <dimension ref="B1:U28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="5.765625" customWidth="1"/>
+    <col min="3" max="3" width="11.07421875" style="53" customWidth="1"/>
+    <col min="4" max="4" width="11.3828125" customWidth="1"/>
+    <col min="7" max="7" width="5.3828125" customWidth="1"/>
+    <col min="8" max="8" width="3.921875" customWidth="1"/>
+    <col min="17" max="17" width="7.765625" customWidth="1"/>
+    <col min="20" max="20" width="5.4609375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
+    </row>
+    <row r="3" spans="2:21" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="42"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="51">
+        <v>-1.8080412582480401E-2</v>
+      </c>
+      <c r="E4" s="51">
+        <v>-0.10231291574887499</v>
+      </c>
+      <c r="F4" s="51">
+        <v>6.8889448787805702E-2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="54">
+        <v>1E-3</v>
+      </c>
+      <c r="D5" s="51">
+        <v>-1.8080412582480401E-2</v>
+      </c>
+      <c r="E5" s="51">
+        <v>-0.10231291574887499</v>
+      </c>
+      <c r="F5" s="51">
+        <v>6.8889448787805702E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="54">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="51">
+        <v>-1.8080412582480401E-2</v>
+      </c>
+      <c r="E6" s="51">
+        <v>-0.10231291574887499</v>
+      </c>
+      <c r="F6" s="51">
+        <v>6.8889448787805702E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="54">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="51">
+        <v>-1.8080412582480401E-2</v>
+      </c>
+      <c r="E7" s="51">
+        <v>-0.10231291574887499</v>
+      </c>
+      <c r="F7" s="51">
+        <v>6.8889448787805702E-2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="54">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="51">
+        <v>-1.8080412582480401E-2</v>
+      </c>
+      <c r="E8" s="51">
+        <v>-0.10231291574887499</v>
+      </c>
+      <c r="F8" s="51">
+        <v>6.8889448787805702E-2</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="I8" s="36"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="30">
+        <v>2</v>
+      </c>
+      <c r="C9" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="31">
+        <v>-1.8080412582480401E-2</v>
+      </c>
+      <c r="E9" s="31">
+        <v>-0.10231291574887499</v>
+      </c>
+      <c r="F9" s="31">
+        <v>6.8889448787805702E-2</v>
+      </c>
+      <c r="G9" s="32">
+        <v>0.95</v>
+      </c>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B10" s="3">
+        <v>24</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="51">
+        <v>0.117168022066999</v>
+      </c>
+      <c r="E10" s="51">
+        <v>-3.5766832860371703E-2</v>
+      </c>
+      <c r="F10" s="51">
+        <v>0.26848311191018098</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.79999999999999905</v>
+      </c>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B11" s="3">
+        <v>24</v>
+      </c>
+      <c r="C11" s="54">
+        <v>1E-3</v>
+      </c>
+      <c r="D11" s="51">
+        <v>-2.3474082059977301E-2</v>
+      </c>
+      <c r="E11" s="51">
+        <v>-0.42298977287740402</v>
+      </c>
+      <c r="F11" s="51">
+        <v>0.374636556540699</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B12" s="3">
+        <v>24</v>
+      </c>
+      <c r="C12" s="54">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D12" s="51">
+        <v>0.863542484168764</v>
+      </c>
+      <c r="E12" s="51">
+        <v>0.60714819441061596</v>
+      </c>
+      <c r="F12" s="51">
+        <v>1.03723266804678</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B13" s="3">
+        <v>24</v>
+      </c>
+      <c r="C13" s="54">
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="51">
+        <v>0.983821066832122</v>
+      </c>
+      <c r="E13" s="51">
+        <v>0.69876555982278898</v>
+      </c>
+      <c r="F13" s="51">
+        <v>1.17984450451319</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B14" s="3">
+        <v>24</v>
+      </c>
+      <c r="C14" s="54">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="51">
+        <v>0.91276501141567001</v>
+      </c>
+      <c r="E14" s="51">
+        <v>0.487261454502805</v>
+      </c>
+      <c r="F14" s="51">
+        <v>1.21045686413415</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B15" s="30">
+        <v>24</v>
+      </c>
+      <c r="C15" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="31">
+        <v>0.99621879221235798</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.82722577301344902</v>
+      </c>
+      <c r="F15" s="31">
+        <v>1.1935302518045401</v>
+      </c>
+      <c r="G15" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.4">
+      <c r="B16" s="3">
+        <v>48</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="51">
+        <v>0.46351265767720401</v>
+      </c>
+      <c r="E16" s="51">
+        <v>0.32109339814694199</v>
+      </c>
+      <c r="F16" s="51">
+        <v>0.73314058561975004</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B17" s="3">
+        <v>48</v>
+      </c>
+      <c r="C17" s="54">
+        <v>1E-3</v>
+      </c>
+      <c r="D17" s="51">
+        <v>0.458806656439886</v>
+      </c>
+      <c r="E17" s="51">
+        <v>9.1844419389381204E-2</v>
+      </c>
+      <c r="F17" s="51">
+        <v>0.77924927833269297</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B18" s="3">
+        <v>48</v>
+      </c>
+      <c r="C18" s="54">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D18" s="51">
+        <v>1.27023283093244</v>
+      </c>
+      <c r="E18" s="51">
+        <v>0.99780093004221204</v>
+      </c>
+      <c r="F18" s="51">
+        <v>1.4777386808442201</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B19" s="3">
+        <v>48</v>
+      </c>
+      <c r="C19" s="54">
+        <v>0.01</v>
+      </c>
+      <c r="D19" s="51">
+        <v>1.20232909084132</v>
+      </c>
+      <c r="E19" s="51">
+        <v>1.0229311351658501</v>
+      </c>
+      <c r="F19" s="51">
+        <v>1.41632800434079</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B20" s="3">
+        <v>48</v>
+      </c>
+      <c r="C20" s="54">
+        <v>0.02</v>
+      </c>
+      <c r="D20" s="51">
+        <v>1.48189991067576</v>
+      </c>
+      <c r="E20" s="51">
+        <v>1.41632800434079</v>
+      </c>
+      <c r="F20" s="51">
+        <v>1.5932338236516801</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B21" s="30">
+        <v>48</v>
+      </c>
+      <c r="C21" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="31">
+        <v>1.70189367949463</v>
+      </c>
+      <c r="E21" s="31">
+        <v>1.56981363934381</v>
+      </c>
+      <c r="F21" s="31">
+        <v>1.8174994963588</v>
+      </c>
+      <c r="G21" s="32">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B22" s="3">
+        <v>72</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="51">
+        <v>0.57786000713797803</v>
+      </c>
+      <c r="E22" s="51">
+        <v>0.16949431807073301</v>
+      </c>
+      <c r="F22" s="51">
+        <v>0.991612592298725</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B23" s="3">
+        <v>72</v>
+      </c>
+      <c r="C23" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="D23" s="51">
+        <v>0.72990548876824701</v>
+      </c>
+      <c r="E23" s="51">
+        <v>0.32679678427048298</v>
+      </c>
+      <c r="F23" s="51">
+        <v>1.0808407616338001</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B24" s="3">
+        <v>72</v>
+      </c>
+      <c r="C24" s="55">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D24" s="51">
+        <v>1.3657639688582801</v>
+      </c>
+      <c r="E24" s="51">
+        <v>0.98572536791415799</v>
+      </c>
+      <c r="F24" s="51">
+        <v>1.7119009632078701</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B25" s="3">
+        <v>72</v>
+      </c>
+      <c r="C25" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="D25" s="51">
+        <v>1.31822510305809</v>
+      </c>
+      <c r="E25" s="51">
+        <v>1.0826805430184401</v>
+      </c>
+      <c r="F25" s="51">
+        <v>1.5537652099011201</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B26" s="3">
+        <v>72</v>
+      </c>
+      <c r="C26" s="55">
+        <v>0.02</v>
+      </c>
+      <c r="D26" s="51">
+        <v>1.53238150643938</v>
+      </c>
+      <c r="E26" s="51">
+        <v>1.3610569681226501</v>
+      </c>
+      <c r="F26" s="51">
+        <v>1.7424809703670401</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B27" s="9">
+        <v>72</v>
+      </c>
+      <c r="C27" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1.76180796491253</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1.55773897074979</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1.9010251543182799</v>
+      </c>
+      <c r="G27" s="11">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.4"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="I7:N9"/>
+    <mergeCell ref="E2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>